<commit_message>
add score file download
</commit_message>
<xml_diff>
--- a/file_store/member_table.xlsx
+++ b/file_store/member_table.xlsx
@@ -1,43 +1,138 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="525" windowWidth="20175" windowHeight="7425"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+  <si>
+    <t>编号</t>
+  </si>
+  <si>
+    <t>用户名</t>
+  </si>
+  <si>
+    <t>中文名</t>
+  </si>
+  <si>
+    <t>昵称</t>
+  </si>
+  <si>
+    <t>密码</t>
+  </si>
+  <si>
+    <t>邮箱</t>
+  </si>
+  <si>
+    <t>部门</t>
+  </si>
+  <si>
+    <t>角色</t>
+  </si>
+  <si>
+    <t>地址</t>
+  </si>
+  <si>
+    <t>修改密码次数</t>
+  </si>
+  <si>
+    <t>raoyuanqin</t>
+  </si>
+  <si>
+    <t>饶源钦</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>******</t>
+  </si>
+  <si>
+    <t>raoyuanqin@qq.com</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>chenmeijing</t>
+  </si>
+  <si>
+    <t>陈美晶</t>
+  </si>
+  <si>
+    <t>chenmeijing@qq.com</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>chenergou</t>
+  </si>
+  <si>
+    <t>陈二狗</t>
+  </si>
+  <si>
+    <t>gaoyuanyuan</t>
+  </si>
+  <si>
+    <t>高圆圆</t>
+  </si>
+  <si>
+    <t>gaoyuanyuan@sina.com</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>fanbingbing</t>
+  </si>
+  <si>
+    <t>范冰冰</t>
+  </si>
+  <si>
+    <t>fanbingbing@sina.com</t>
+  </si>
+  <si>
+    <t>goudan</t>
+  </si>
+  <si>
+    <t>苟丹</t>
+  </si>
+  <si>
+    <t>goudan@163.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -53,16 +148,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -350,17 +444,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>